<commit_message>
Add CoordinateFormatter to template
</commit_message>
<xml_diff>
--- a/templates/export/prior-notification-report.xlsx
+++ b/templates/export/prior-notification-report.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27218"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{600EB3C8-12F1-45D8-8D0D-AE661361AC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{003E78DA-5AC3-49CC-B352-7B875D724FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -154,7 +154,7 @@
     <t>${speedUnit.equals("kmh") ? "".format("%.1f km/h", position.speed * 1.852) : speedUnit.equals("mph") ? "".format("%.1f mph", position.speed * 1.15078) : "".format("%.1f kn", position.speed)}</t>
   </si>
   <si>
-    <t>${position.attributes.toString().replaceAll(",", " ").replaceAll(bracketsRegex, "")}</t>
+    <t>${position.fishes.toString()}</t>
   </si>
 </sst>
 </file>
@@ -1032,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Rename title of report in prior-notification-report.xlsx
</commit_message>
<xml_diff>
--- a/templates/export/prior-notification-report.xlsx
+++ b/templates/export/prior-notification-report.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27218"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{003E78DA-5AC3-49CC-B352-7B875D724FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEB75A31-5927-424C-8B62-45293464969C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,7 +91,7 @@
     <t>Report type:</t>
   </si>
   <si>
-    <t>Route</t>
+    <t>Prior Notification</t>
   </si>
   <si>
     <t>Device:</t>
@@ -1032,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>